<commit_message>
still need to enter the rankings
</commit_message>
<xml_diff>
--- a/experimental results/e3000_CartPole.xlsx
+++ b/experimental results/e3000_CartPole.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="78">
   <si>
     <t>01_i_domain_name</t>
   </si>
@@ -70,13 +70,13 @@
     <t>[0,0]</t>
   </si>
   <si>
-    <t>[9, 13]</t>
-  </si>
-  <si>
-    <t>[1, 0, 1, 0, 1, 0, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 0, 1, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 0, 1, 0]</t>
-  </si>
-  <si>
-    <t>['[-0.01881685 -0.00766736  0.03277026 -0.00908009]', '(-0.018970201901006303, 0.186969673090352, 0.032588657654782506, -0.2912461466670848)', '(-0.015230808439199262, -0.008601427704964998, 0.02676373472144081, 0.011534112466383584)', '(-0.015402836993298563, 0.18612667547570355, 0.026994416970768483, -0.27258583743663833)', '(-0.011680303483784491, -0.009369849307344524, 0.021542700222035718, 0.028487507456279093)', '(-0.011867700469931382, 0.1854366465508055, 0.0221124503711613, -0.2573213694562454)', '(-0.008158967538915273, -0.009993906974345684, 0.01696602298203639, 0.04225332601995413)', '(-0.008358845678402187, 0.1848806988513335, 0.017811089502435474, -0.2450287418665169)', '(-0.004661231701375517, -0.010491057663022746, 0.012910514665105136, 0.05321859353121916)', '(-0.004871052854635972, -0.205795726467411, 0.013974886535729519, 0.34994676770407274)', '(-0.008986967383984194, -0.010875285114496508, 0.02097382188981097, 0.06170313871853211)', '(-0.009204473086274124, 0.18393976714461902, 0.022207884664181613, -0.22428931594269658)', '(-0.005525677743381745, -0.01149243166815972, 0.017722098345327682, 0.07531527774385866)', '(-0.0057555263767449395, -0.20686390308079405, 0.019228403900204853, 0.37353648960532637)', '(-0.009892804438360821, -0.012020300570695697, 0.02669913369231138, 0.08697791643607211)', '(-0.010133210449774735, 0.18270897044573678, 0.028438692021032823, -0.19716327486092305)', '(-0.006479031040859999, 0.37741284848650375, 0.02449542652381436, -0.48074114996933276)', '(0.0010692259288700764, 0.18195383985290986, 0.014880603524427705, -0.18043965775155968)', '(0.004708302725928273, 0.3768597278954582, 0.011271810369396512, -0.4683913855787544)', '(0.012245497283837437, 0.1815803640334391, 0.0019039826578214226, -0.1721771057394012)', '(0.01587710456450622, -0.013568786186731407, -0.0015395594569666015, 0.12110585957050468)', '(0.01560572884077159, 0.18157518865984595, 0.0008825577344434921, -0.1720623860969434)', '(0.019237232613968508, -0.013559383109949946, -0.002558689987495376, 0.12089882950406822)', '(0.01896604495176951, 0.18159913333256222, -0.00014071339741401163, -0.17259024093406816)', '(0.022598027618420752, -0.013520803657499636, -0.003592518216095375, 0.12004829191475236)', '(0.02232761154527076, 0.18165243426419286, -0.0011915523778003277, -0.17376587384668296)', '(0.025960660230554617, -0.01345244319858685, -0.004666869854733987, 0.11854091827433444)', '(0.02569161136658288, 0.18173606175658252, -0.0022960514892472984, -0.17561070556446112)', '(0.029326332601714532, -0.013352954666806721, -0.0058082656005365215, 0.11634700916585983)', '(0.0290592735083784, 0.18185173514740494, -0.003481325417219325, -0.17816270699285963)', '(0.0326963082113265, -0.013220223993525071, -0.007044579557076517, 0.11341995096560087)', '(0.032431903731456, 0.1820019561777085, -0.004776180537764499, -0.1814771424942227)', '(0.03607194285501017, -0.013051326553097903, -0.008405723387648953, 0.10969525271689318)', '(0.035810916323948214, 0.18219006131685384, -0.00621181833331109, -0.1856277364643098)', '(0.03945471755028529, -0.012842463800842752, -0.009924373062597285, 0.10508914414109738)', '(0.03919786827426844, 0.1824202940022731, -0.007822590179775338, -0.19070828642837012)', '(0.0428462741543139, -0.012588878824211919, -0.01163675590834274, 0.09949670491462631)', '(0.04259449657782966, 0.18269789816995283, -0.009646821810050214, -0.19683475638913805)', '(0.046248454541228716, -0.012284749060034517, -0.013583516937832975, 0.09278948395339237)', '(0.04600275956002803, 0.18302923486500505, -0.011727727258765128, -0.20414789520043153)', '(0.04966334425732813, -0.011923053956696739, -0.015810685162773758, 0.08481255524339049)', '(0.04942488317819419, 0.18342192412084068, -0.014114434057905948, -0.21281643648663418)', '(0.053093321660611, -0.011495414887692762, -0.01837076278763863, 0.07538094350333796)', '(0.052863413362857145, 0.1838850146601135, -0.01686314391757187, -0.2230409492186764)', '(0.05654111365605941, -0.010991904171996802, -0.0213239629019454, 0.06427533844660849)', '(0.05632127557261948, 0.1844291842631839, -0.02003845613301323, -0.23505842157262968)', '(0.06000985925788316, -0.010400819666470273, -0.024739624564465823, 0.051237000450171155)', '(0.059801842864553756, -0.20515945626926496, -0.0237148845554624, 0.33601285084571075)', '(0.055698653739168456, -0.009708179862454758, -0.016994627538548183, 0.03594685053986696)', '(0.05550449014191936, -0.204582353726972, -0.016275690527750845, 0.3232197200775537)']</t>
+    <t>[19, 21, 22, 28]</t>
+  </si>
+  <si>
+    <t>[1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 0, 1, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1]</t>
+  </si>
+  <si>
+    <t>['[-0.01881685 -0.00766736  0.03277026 -0.00908009]', '(-0.018970201901006303, 0.186969673090352, 0.032588657654782506, -0.2912461466670848)', '(-0.015230808439199262, -0.008601427704964998, 0.02676373472144081, 0.011534112466383584)', '(-0.015402836993298563, 0.18612667547570355, 0.026994416970768483, -0.27258583743663833)', '(-0.011680303483784491, -0.009369849307344524, 0.021542700222035718, 0.028487507456279093)', '(-0.011867700469931382, 0.1854366465508055, 0.0221124503711613, -0.2573213694562454)', '(-0.008158967538915273, -0.009993906974345684, 0.01696602298203639, 0.04225332601995413)', '(-0.008358845678402187, 0.1848806988513335, 0.017811089502435474, -0.2450287418665169)', '(-0.004661231701375517, -0.010491057663022746, 0.012910514665105136, 0.05321859353121916)', '(-0.004871052854635972, 0.18444341680172113, 0.013974886535729519, -0.23536316367543225)', '(-0.0011821845186015495, -0.010875382469220513, 0.009267623262220873, 0.06169490965754798)', '(-0.0013996921679859597, 0.18411247411902293, 0.010501521455371832, -0.22804967261799397)', '(0.0022825573143944993, -0.011157964735623443, 0.005940528003011952, 0.06792722526830997)', '(0.0020593980196820304, 0.1838783157507662, 0.007299072508378151, -0.22287552841176522)', '(0.005736964334697355, -0.011347196378286711, 0.0028415619401428466, 0.07210084738632738)', '(0.00551002040713162, 0.18373390205906265, 0.004283578887869394, -0.21968420080137002)', '(0.009184698448312873, -0.011449017457679123, -0.00011010512815800687, 0.0743468607539246)', '(0.00895571809915929, 0.18367451206364416, 0.0013768320869204853, -0.21837080266154113)', '(0.012629208340432173, -0.011467093796386357, -0.002990583966310337, 0.0747461171916447)', '(0.012399866464504446, -0.20654604456079387, -0.001495661622477443, 0.3664840044337423)', '(0.00826894557328857, -0.011402871321903624, 0.0058340184661974034, 0.07332984762428052)', '(0.008040888146850497, -0.2066079722619717, 0.0073006154186830135, 0.36784770778074066)', '(0.003908728701611063, -0.4018328961632578, 0.014657569574297827, 0.6628236515660311)', '(-0.004127929221654093, -0.20691790744245622, 0.027914042605618448, 0.3747917463607584)', '(-0.008266287370503219, -0.012203350206742597, 0.03540987753283362, 0.09103935619238201)', '(-0.008510354374638072, 0.18239363620813515, 0.037230664656681255, -0.19026481602126982)', '(-0.004862481650475369, 0.37696372820084506, 0.03342536833625586, -0.4709744170254129)', '(0.0026767929135415322, 0.18138597998628522, 0.024005879995747603, -0.16794643364081968)', '(0.006304512513267237, -0.014071217638710998, 0.02064695132293121, 0.1322119388290675)', '(0.006023088160493017, 0.18074898625776922, 0.02329119009951256, -0.15388630842205253)', '(0.009638067885648402, 0.3755298364136519, 0.02021346393107151, -0.4391313479780772)', '(0.01714866461392144, 0.1801277170825535, 0.011430836971509966, -0.14014569187761794)', '(0.02075121895557251, 0.3750841028275297, 0.008627923133957608, -0.4292005724785327)', '(0.0282529010121231, 0.17984103474129248, 4.3911684386954e-05, -0.13381029292672875)', '(0.03184972170694895, 0.3749623569425311, -0.002632294174147621, -0.42647936591120106)', '(0.03934896884579957, 0.17987778831053605, -0.011161881492371642, -0.1346274203578331)', '(0.04294652461201029, -0.015082518638370929, -0.013854429899528304, 0.15451329800912322)', '(0.04264487423924287, 0.18023503425323142, -0.01076416393934584, -0.1425079861603074)', '(0.04624957492430749, -0.014731115418976204, -0.013614323662551987, 0.1467596927864553)', '(0.04595495261592797, 0.18058312620635839, -0.010679129806822882, -0.1501870064886447)', '(0.049566615140055136, -0.014384290431230184, -0.013682869936595775, 0.139107838018455)', '(0.049278929331430535, 0.18093093488986606, -0.010900713176226675, -0.15786021330578975)', '(0.05289754802922786, -0.01403326648840214, -0.01405791744234247, 0.13136396768233627)', '(0.05261688269945981, 0.18128720839278428, -0.011430638088695745, -0.16572068655106853)', '(0.0562426268673155, -0.01366926749762934, -0.014745051819717116, 0.1233343883916958)', '(0.05596924151736291, 0.18166079269111, -0.012278364051883199, -0.17396373962878042)', '(0.059602457371185115, -0.013283298692020162, -0.015757638844458806, 0.11482060732433147)', '(0.05933679139734471, 0.1820608512301758, -0.013461226697972176, -0.1827917939829249)', '(0.06297800842194823, -0.01286592406050549, -0.017117062577630675, 0.10561439700062603)', '(0.06272068994073812, 0.18249708877857318, -0.015004774637618155, -0.1924193638448825)']</t>
   </si>
   <si>
     <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38, 39, 40, 41, 42, 43, 44, 45, 46, 47, 48, 49]</t>
@@ -85,160 +85,169 @@
     <t>Omitted</t>
   </si>
   <si>
+    <t>['[0,0]', '[1,0]', '[1,1]']</t>
+  </si>
+  <si>
+    <t>[1, 2, 5, 12, 13, 14, 22, 25, 26, 31, 35, 36, 39, 40, 43, 48]</t>
+  </si>
+  <si>
+    <t>[1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 0, 1, 1, 1, 1, 1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 1]</t>
+  </si>
+  <si>
+    <t>['[-0.01881685 -0.00766736  0.03277026 -0.00908009]', '(-0.018970201901006303, -0.203243578415405, 0.032588657654782506, 0.29375947416390885)', '(-0.023035073469314403, -0.3988146324758434, 0.03846384713806068, 0.5965396632322811)', '(-0.03101136611883127, -0.2042514664103063, 0.0503946404027063, 0.31621635780497453)', '(-0.035096395447037396, -0.009882199210565407, 0.056718967558805795, 0.039842350584417374)', '(-0.0352940394312487, -0.20576969102121356, 0.05751581457049414, 0.3498675183875401)', '(-0.039409433251672975, -0.011510887231409084, 0.06451316493824495, 0.07586147396499004)', '(-0.03963965099630116, 0.18262973753309925, 0.06603039441754475, -0.19578995417103678)', '(-0.03598705624563917, 0.3767480953442379, 0.06211459533412402, -0.4669341203085862)', '(-0.028452094338754414, 0.5709399741453058, 0.0527759129279523, -0.739410242136233)', '(-0.0170332948558483, 0.37513055032793163, 0.03798770808522764, -0.430596135454884)', '(-0.009530683849289666, 0.179491841319433, 0.02937578537612996, -0.12618408590119085)', '(-0.005940847022901007, -0.016038360506487825, 0.02685210365810614, 0.1756199171189224)', '(-0.0062616142330307635, -0.21153410559505698, 0.03036450200048459, 0.47665139138400225)', '(-0.010492296344931904, -0.4070713435745349, 0.039897529828164635, 0.7787478361440401)', '(-0.0186337232164226, -0.21252002309077558, 0.05547248655104543, 0.49887985364028015)', '(-0.02288412367823811, -0.018222238418754144, 0.06545008362385103, 0.2241820290849833)', '(-0.023248568446613195, 0.17590618672125152, 0.0699337242055507, -0.04715854890103477)', '(-0.019730444712188166, 0.36995927420485575, 0.06899055322753, -0.31698291514289867)', '(-0.01233125922809105, 0.5640342107244563, 0.06265089492467203, -0.5871356551883224)', '(-0.001050575013601925, 0.7582253630047998, 0.05090818182090558, -0.8594435850354614)', '(0.01411393224649407, 0.5624483383444254, 0.033719310120196355, -0.5511979625429878)', '(0.02536289901338258, 0.36686942708478487, 0.0226953508693366, -0.24808475988508777)', '(0.032700287555078277, 0.5616600279942232, 0.017733655671634842, -0.5335235547099824)', '(0.04393348811496274, 0.3662932230789822, 0.007063184577435195, -0.2353060042143968)', '(0.051259352576542384, 0.17107107298828275, 0.002357064493147259, 0.05959647543523139)', '(0.05468077403630804, -0.02408459435849039, 0.003548994001851887, 0.35302213959756806)', '(0.05419908214913823, 0.17098671124509726, 0.010609436793803249, 0.06146042598121593)', '(0.05761881637404018, 0.36595495241082643, 0.011838645313427567, -0.2278563607791284)', '(0.0649379154222567, 0.5609057364813291, 0.0072815180978449984, -0.5167815644242888)', '(0.07615603015188328, 0.365682015872987, -0.003054113190640778, -0.2218129992193869)', '(0.08346967046934302, 0.17060385137545556, -0.007490373175028517, 0.06990497493641762)', '(0.08688174749685212, 0.3658323843240716, -0.006092273676300164, -0.22513175857235085)', '(0.09419839518333356, 0.5610408741134525, -0.010594908847747182, -0.5197301766649856)', '(0.10541921266560261, 0.3660696673336875, -0.02098951238104689, -0.23040462571222164)', '(0.11274060601227637, 0.17125384021020956, -0.025597604895291323, 0.055584282804146234)', '(0.11616568281648056, -0.023491906495457265, -0.024485919239208398, 0.34008233055586934)', '(0.11569584468657142, 0.1719697324581838, -0.01768427262809101, 0.03977962008507574)', '(0.1191352393357351, 0.367340751656247, -0.016888680226389497, -0.25842999077364004)', '(0.12648205436886004, 0.17246392915927433, -0.022057280041862297, 0.028878519836912808)', '(0.12993133295204554, -0.022334875348822864, -0.02147970964512404, 0.31452133431161217)', '(0.12948463544506908, 0.17308636244956865, -0.015189282958891798, 0.015142548254282906)', '(0.13294636269406046, 0.3684228159877024, -0.01488643199380614, -0.2822938099924707)', '(0.1403148190138145, 0.1735163293160605, -0.020532308193655556, 0.005657076938019923)', '(0.14378514560013572, 0.368926633514429, -0.020419166654895158, -0.2934326708339356)', '(0.1511636782704243, 0.1741016693792489, -0.02628782007157387, -0.007258963438733446)', '(0.15464571165800928, 0.3695905688543466, -0.026432999340348536, -0.30811872809737995)', '(0.16203752303509622, 0.17485503445677517, -0.03259537390229614, -0.02388786421745903)', '(0.16553462372423172, -0.01978467448145843, -0.033073131186645316, 0.25833527238896964)', '(0.16513893023460255, 0.1757934473745177, -0.027906425738865922, -0.044593205832358096)']</t>
+  </si>
+  <si>
+    <t>[7, 8, 10, 11, 12, 13, 17]</t>
+  </si>
+  <si>
+    <t>[1, 0, 1, 0, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1]</t>
+  </si>
+  <si>
+    <t>['[-0.01881685 -0.00766736  0.03277026 -0.00908009]', '(-0.018970201901006303, 0.186969673090352, 0.032588657654782506, -0.2912461466670848)', '(-0.015230808439199262, -0.008601427704964998, 0.02676373472144081, 0.011534112466383584)', '(-0.015402836993298563, 0.18612667547570355, 0.026994416970768483, -0.27258583743663833)', '(-0.011680303483784491, -0.009369849307344524, 0.021542700222035718, 0.028487507456279093)', '(-0.011867700469931382, 0.1854366465508055, 0.0221124503711613, -0.2573213694562454)', '(-0.008158967538915273, -0.009993906974345684, 0.01696602298203639, 0.04225332601995413)', '(-0.008358845678402187, -0.20535498527219764, 0.017811089502435474, 0.3402405405228112)', '(-0.01246594538384614, -0.4007257735531117, 0.024615900312891698, 0.6384864238007459)', '(-0.020480460854908372, -0.20595555231548998, 0.03738562878890662, 0.3536559459868527)', '(-0.02459957190121817, -0.40158860989834333, 0.04445874770864367, 0.6578892957972458)', '(-0.032631344099185035, -0.5973002710173932, 0.05761653362458859, 0.9642332717227169)', '(-0.0445773495195329, -0.7931469478962471, 0.07690119905904293, 1.274445703235819)', '(-0.06044028847745784, -0.9891610430382135, 0.10239011312375931, 1.5901845590132704)', '(-0.08022350933822212, -0.7953932389350284, 0.13419380430402472, 1.3311052027580068)', '(-0.09613137411692269, -0.6021945715524115, 0.16081590835918486, 1.083247299826135)', '(-0.10817526554797091, -0.4095175617128118, 0.18248085435570754, 0.8450373124612733)', '(-0.11636561678222715, -0.6065975341354181, 0.199381600604933, 1.1891010699445699)', '(-0.1284975674649355, -0.4145378947655146, 0.22316362200382442, 0.9649494666397327)']</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18]</t>
+  </si>
+  <si>
+    <t>['[1,0]', '[0,0]', '[1,1]']</t>
+  </si>
+  <si>
+    <t>[1, 3, 6, 7, 12, 13, 14, 15, 16, 18, 22]</t>
+  </si>
+  <si>
+    <t>[1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1]</t>
+  </si>
+  <si>
+    <t>['[-0.01881685 -0.00766736  0.03277026 -0.00908009]', '(-0.018970201901006303, -0.203243578415405, 0.032588657654782506, 0.29375947416390885)', '(-0.023035073469314403, -0.008601042343346021, 0.03846384713806068, 0.01153006168279358)', '(-0.023207094316181322, -0.20425290291665268, 0.03869444837171655, 0.31609636674495395)', '(-0.027292152374514374, -0.009702865384165815, 0.04501637570661563, 0.035863081415907105)', '(-0.02748620968219769, 0.18474560036540177, 0.045733637334933776, -0.24228378862138145)', '(-0.023791297674889657, -0.010998769621198362, 0.040887961562506146, 0.06446676351011005)', '(-0.024011273067313623, -0.20668237058004738, 0.04217729683270835, 0.3697645489792695)', '(-0.02814492047891457, -0.012184263883037894, 0.04957258781229374, 0.09067329764822685)', '(-0.02838860575657533, 0.18219338254328513, 0.051386053765258274, -0.18596661929979075)', '(-0.024744738105709627, 0.37654389488832274, 0.04766672137926246, -0.4620067296819313)', '(-0.017213860207943174, 0.18078181198539575, 0.03842658678562383, -0.15468842806098887)', '(-0.013598223968235259, -0.014868665066518044, 0.03533281822440405, 0.149865277100259)', '(-0.013895597269565619, -0.2104782840302001, 0.038330123766409235, 0.45348226144649967)', '(-0.01810516295016962, -0.40612069703284226, 0.04739976899533923, 0.7579966263815202)', '(-0.026227576890826467, -0.6018626977941299, 0.06255970152296964, 1.0652101679374133)', '(-0.038264830846709064, -0.7977542750881016, 0.08386390488171791, 1.3768532807379537)', '(-0.05421991634847109, -0.6037740925497065, 0.11140097049647699, 1.1115327234519108)', '(-0.06629539819946523, -0.800168907389127, 0.1336316249655152, 1.436983049256065)', '(-0.08229877634724778, -0.6069232901330598, 0.1623712859506365, 1.188869796698075)', '(-0.09443724214990898, -0.4142348108349193, 0.186148681884598, 0.9511664801646266)', '(-0.10272193836660737, -0.22203960307703274, 0.20517201148789052, 0.7222663218198737)', '(-0.10716273042814803, -0.41931927226406, 0.219617337924288, 1.071877452947799)']</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22]</t>
+  </si>
+  <si>
+    <t>['[1,1]', '[0,0]', '[1,0]']</t>
+  </si>
+  <si>
+    <t>[1, 2, 3, 4, 5, 6, 7, 8, 9]</t>
+  </si>
+  <si>
+    <t>[1, 1, 1, 1, 1, 1, 1, 1, 1]</t>
+  </si>
+  <si>
+    <t>['[-0.01881685 -0.00766736  0.03277026 -0.00908009]', '(-0.018970201901006303, -0.203243578415405, 0.032588657654782506, 0.29375947416390885)', '(-0.023035073469314403, -0.3988146324758434, 0.03846384713806068, 0.5965396632322811)', '(-0.03101136611883127, -0.5944531488919764, 0.0503946404027063, 0.9010859668635411)', '(-0.0429004290966708, -0.7902203588335466, 0.06841635973997713, 1.209173733871254)', '(-0.058704836273341734, -0.9861559232896362, 0.09259983441740222, 1.5224882192013063)', '(-0.07842795473913446, -1.182266511478129, 0.12304959880142835, 1.8425792671068442)', '(-0.10207328496869704, -1.3785125418350686, 0.15990118414356524, 2.1708079305885084)', '(-0.12964353580539842, -1.5747927147279073, 0.20331734275533542, 2.508283148799749)', '(-0.16113939009995656, -1.770926329198504, 0.2534830057313304, 2.8557879869215794)']</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9]</t>
+  </si>
+  <si>
     <t>['[1,0]', '[1,1]', '[0,0]']</t>
   </si>
   <si>
-    <t>[1, 3, 4, 7, 8, 9, 11, 12, 15]</t>
-  </si>
-  <si>
-    <t>[1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1]</t>
-  </si>
-  <si>
-    <t>['[-0.01881685 -0.00766736  0.03277026 -0.00908009]', '(-0.018970201901006303, -0.203243578415405, 0.032588657654782506, 0.29375947416390885)', '(-0.023035073469314403, -0.008601042343346021, 0.03846384713806068, 0.01153006168279358)', '(-0.023207094316181322, -0.20425290291665268, 0.03869444837171655, 0.31609636674495395)', '(-0.027292152374514374, -0.39990404041704386, 0.04501637570661563, 0.6207267240778034)', '(-0.03529023318285525, -0.20543871750851112, 0.0574309101881717, 0.34255459391818766)', '(-0.03939900753302547, -0.011178859621362947, 0.06428200206653545, 0.06852062916750595)', '(-0.03962258472545273, -0.20716070266072686, 0.06565241464988557, 0.38077212496967605)', '(-0.043765798778667264, -0.40315049926572394, 0.0732678571492791, 0.6934114221766585)', '(-0.05182880876398174, -0.5992082511848367, 0.08713608559281226, 1.0082305310355233)', '(-0.06381297378767847, -0.4053507641855476, 0.10730069621352273, 0.744133131332519)', '(-0.07191998907138943, -0.6017770796219798, 0.1221833588401731, 1.0685639793074835)', '(-0.08395553066382902, -0.7982845712250702, 0.14355463842632277, 1.39696033658418)', '(-0.09992122208833043, -0.6052100013634932, 0.17149384515800636, 1.1523877646982918)', '(-0.11202542211560029, -0.4126887349220147, 0.1945416004519722, 0.9180144398825633)', '(-0.12027919681404059, -0.6098328006206857, 0.21290188924962344, 1.2649874049973338)']</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15]</t>
-  </si>
-  <si>
-    <t>['[0,0]', '[1,0]', '[1,1]']</t>
-  </si>
-  <si>
-    <t>[1, 2, 4, 8, 10, 11, 12, 13, 14, 16, 17]</t>
-  </si>
-  <si>
-    <t>[1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1]</t>
-  </si>
-  <si>
-    <t>['[-0.01881685 -0.00766736  0.03277026 -0.00908009]', '(-0.018970201901006303, -0.203243578415405, 0.032588657654782506, 0.29375947416390885)', '(-0.023035073469314403, -0.3988146324758434, 0.03846384713806068, 0.5965396632322811)', '(-0.03101136611883127, -0.2042514664103063, 0.0503946404027063, 0.31621635780497453)', '(-0.035096395447037396, -0.40005365906793083, 0.056718967558805795, 0.6243565322687714)', '(-0.043097468628396016, -0.2057675226194045, 0.06920609820418122, 0.35006240883399925)', '(-0.047212819080784105, -0.011694559111823488, 0.07620734638086121, 0.07998017254192302)', '(-0.047446710263020574, 0.18225690997682453, 0.07780694983169967, -0.18771937153962787)', '(-0.04380157206348408, -0.01388702574823203, 0.07405256240090712, 0.1284585706804547)', '(-0.04407931257844872, 0.18010027711004498, 0.07662173381451622, -0.13997334959462487)', '(-0.04047730703624782, -0.016030694228310688, 0.07382226682262372, 0.1758646864648018)', '(-0.04079792092081404, -0.21212724337962996, 0.07733956055191975, 0.49089240818620944)', '(-0.04504046578840663, -0.40825011030541214, 0.08715740871564394, 0.8069124991324104)', '(-0.05320546799451488, -0.6044516312379551, 0.10329565869829214, 1.1256895153801452)', '(-0.06529450061927398, -0.8007642806410986, 0.12580944900589505, 1.4489038413260646)', '(-0.08130978623209595, -0.6073934216590353, 0.15478752583241634, 1.1980305154761164)', '(-0.09345765466527665, -0.8041419084981484, 0.17874813614193866, 1.5349508795859683)', '(-0.10954049283523962, -1.0009092873938221, 0.20944715373365802, 1.877671870249867)']</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17]</t>
+    <t>[1,1]</t>
+  </si>
+  <si>
+    <t>[14, 15, 18, 21, 28, 30, 45]</t>
+  </si>
+  <si>
+    <t>[1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 0, 1, 0, 0, 0, 0, 0, 1, 0, 1, 0, 1, 1, 0, 1, 0, 1, 0, 1, 0, 0, 0, 1, 0]</t>
+  </si>
+  <si>
+    <t>['[-0.01881685 -0.00766736  0.03277026 -0.00908009]', '(-0.018970201901006303, 0.186969673090352, 0.032588657654782506, -0.2912461466670848)', '(-0.015230808439199262, -0.008601427704964998, 0.02676373472144081, 0.011534112466383584)', '(-0.015402836993298563, 0.18612667547570355, 0.026994416970768483, -0.27258583743663833)', '(-0.011680303483784491, -0.009369849307344524, 0.021542700222035718, 0.028487507456279093)', '(-0.011867700469931382, 0.1854366465508055, 0.0221124503711613, -0.2573213694562454)', '(-0.008158967538915273, -0.009993906974345684, 0.01696602298203639, 0.04225332601995413)', '(-0.008358845678402187, 0.1848806988513335, 0.017811089502435474, -0.2450287418665169)', '(-0.004661231701375517, -0.010491057663022746, 0.012910514665105136, 0.05321859353121916)', '(-0.004871052854635972, 0.18444341680172113, 0.013974886535729519, -0.23536316367543225)', '(-0.0011821845186015495, -0.010875382469220513, 0.009267623262220873, 0.06169490965754798)', '(-0.0013996921679859597, 0.18411247411902293, 0.010501521455371832, -0.22804967261799397)', '(0.0022825573143944993, -0.011157964735623443, 0.005940528003011952, 0.06792722526830997)', '(0.0020593980196820304, 0.1838783157507662, 0.007299072508378151, -0.22287552841176522)', '(0.005736964334697355, 0.37889518481465034, 0.0028415619401428466, -0.5132471314229992)', '(0.013314868030990362, 0.5739769991137685, -0.007423380688317136, -0.8050332533990147)', '(0.024794408013265733, 0.3789575989155256, -0.02352404575629743, -0.5146946670815349)', '(0.03237355999157625, 0.1841746988277678, -0.03381793909792813, -0.2295165866494141)', '(0.0360570539681316, 0.3797631804300992, -0.03840827083091641, -0.5326721401046928)', '(0.04365231757673359, 0.1852018797683274, -0.04906171363301027, -0.25233468008693377)', '(0.047356355172100136, -0.009186420390773858, -0.05410840723474895, 0.024478555620511433)', '(0.04717262676428466, 0.18666806356505286, -0.05361883612233872, -0.284773330513157)', '(0.050905988035585714, -0.0076497898698496825, -0.05931430273260186, -0.009471830289263072)', '(0.05075299223818872, -0.2018731461671734, -0.059503739338387124, 0.26392268735513885)', '(0.04671552931484525, -0.39609752150944577, -0.054225285591284346, 0.5372598579284669)', '(0.038793578884656336, -0.20025678049369736, -0.04348008843271501, 0.22799610306905904)', '(0.03478844327478239, -0.3947312687774748, -0.03892016637133383, 0.5066530171946757)', '(0.02689381789923289, -0.1990831276877706, -0.028787106027440317, 0.20196341001251727)', '(0.022912155345477477, -0.0035615531434651237, -0.02474783782718997, -0.09965967930581476)', '(0.022840924282608175, -0.19832024272864332, -0.026741031413306266, 0.1851137772146948)', '(0.018874519428035308, -0.0028260890942557737, -0.02303875586901237, -0.11588353989869943)', '(0.018817997646150192, -0.19761048588557129, -0.02535642666698636, 0.16944272230780222)', '(0.014865787928438765, -0.3923604948116086, -0.021967572220830317, 0.45401983945232643)', '(0.007018578032206593, -0.1969349146956083, -0.012887175431783788, 0.15449425014827728)', '(0.0030798797382944262, -0.39186999676138506, -0.009797290428818243, 0.4430838678694195)', '(-0.004757520196933275, -0.1966107948899114, -0.0009356130714298534, 0.1473287643877182)', '(-0.008689736094731504, -0.3917193353724826, 0.0020109622163245106, 0.4397163768143268)', '(-0.016524122802181157, -0.19662590260752377, 0.010805289752611046, 0.14766804187365834)', '(-0.02045664085433163, -0.001660338652241966, 0.013758650590084211, -0.14158653855536762)', '(-0.020489847627376472, -0.19697660987003895, 0.010926919818976859, 0.1554050542661537)', '(-0.02442937982477725, -0.0020127999619889425, 0.014035020904299932, -0.1338107516153697)', '(-0.024469635824017028, -0.19733294730084378, 0.011358805871992539, 0.16326677465885758)', '(-0.028416294770033903, -0.0023754290291708724, 0.01462414136516969, -0.1258112204106424)', '(-0.02846380335061732, -0.19770379969520543, 0.012107916956956842, 0.17144934995610128)', '(-0.03241787934452143, -0.0027572206116708575, 0.015536903956078867, -0.11738944370400972)', '(-0.03247302375675484, 0.19213871121287782, 0.013189115081998673, -0.40513039092783165)', '(-0.028630249532497286, -0.0031677716394359068, 0.0050865072634420395, -0.10831865944058539)', '(-0.028693604965286005, -0.19836224181258566, 0.002920134074630332, 0.18596468487940365)', '(-0.03266084980153772, -0.0032821925455689682, 0.006639427772218405, -0.1057956232117297)', '(-0.0327264936524491, -0.19849865791327687, 0.004523515307983811, 0.1889745981379844)']</t>
+  </si>
+  <si>
+    <t>['[1,1]', '[1,0]', '[0,0]']</t>
+  </si>
+  <si>
+    <t>[8, 12, 20, 23, 25, 31, 34, 38, 40, 47, 49]</t>
+  </si>
+  <si>
+    <t>[1, 0, 1, 0, 1, 0, 1, 0, 0, 0, 1, 0, 0, 0, 0, 1, 0, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 0, 0, 1, 0, 1, 1, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>['[-0.01881685 -0.00766736  0.03277026 -0.00908009]', '(-0.018970201901006303, 0.186969673090352, 0.032588657654782506, -0.2912461466670848)', '(-0.015230808439199262, -0.008601427704964998, 0.02676373472144081, 0.011534112466383584)', '(-0.015402836993298563, 0.18612667547570355, 0.026994416970768483, -0.27258583743663833)', '(-0.011680303483784491, -0.009369849307344524, 0.021542700222035718, 0.028487507456279093)', '(-0.011867700469931382, 0.1854366465508055, 0.0221124503711613, -0.2573213694562454)', '(-0.008158967538915273, -0.009993906974345684, 0.01696602298203639, 0.04225332601995413)', '(-0.008358845678402187, 0.1848806988513335, 0.017811089502435474, -0.2450287418665169)', '(-0.004661231701375517, 0.3797437874814581, 0.012910514665105136, -0.532040829553236)', '(0.002933644048253645, 0.18444264827351967, 0.0022696980740404167, -0.23531794933382472)', '(0.006622497013724039, -0.010711657446601935, -0.002436660912636078, 0.058080045900171184)', '(0.006408263864792, 0.18444514611551735, -0.0012750599946326543, -0.2353706680120906)', '(0.010097166787102346, 0.379585291413127, -0.005982473354874467, -0.5284555155544692)', '(0.017688872615364885, 0.1845480163844057, -0.01655158366596385, -0.23766367495682322)', '(0.021379832943052998, -0.010333610170808055, -0.021304857165100315, 0.049752780788707485)', '(0.021173160739636838, -0.20514369340755884, -0.020309801549326167, 0.3356384361998935)', '(0.017070286871485662, -0.009738678922365351, -0.013597032825328297, 0.036620692903581)', '(0.016875513293038356, -0.20466303388981794, -0.012864618967256677, 0.32498279318710427)', '(0.012782252615241997, -0.00936029598525065, -0.006364963103514591, 0.02827083406440062)', '(0.012595046695536984, 0.18585235202093012, -0.005799546422226579, -0.2664134930304255)', '(0.016312093735955588, 0.38105659336322517, -0.011127816282835089, -0.5609199879148371)', '(0.02393322560322009, 0.18609256886524334, -0.02234621604113183, -0.27176356799669504)', '(0.027655076980524957, -0.008703505309238246, -0.02778148740106573, 0.013788351488036699)', '(0.027481006874340193, 0.18680562462962685, -0.027505720371304995, -0.28752888529560283)', '(0.03121711936693273, -0.00791349485523532, -0.03325629807721705, -0.0036463494496517534)', '(0.031058849469828023, 0.187669226543544, -0.03332922506621008, -0.3066337628390033)', '(0.034812234000698904, -0.006962331524712706, -0.03946190032299015, -0.024645541840651597)', '(0.03467298737020465, -0.20149679744847931, -0.039954811159803184, 0.2553301958632065)', '(0.03064305142123506, -0.3960261777738108, -0.03484820724253906, 0.5351477998661018)', '(0.022722527865758846, -0.20043196448563066, -0.02414525124521702, 0.23169130935998333)', '(0.018713888576046233, -0.0049734702555079835, -0.019511425058017354, -0.0685089870504999)', '(0.018614419170936074, 0.1904227007798862, -0.020881604799027353, -0.36728345051686995)', '(0.022422873186533798, -0.004396397789137418, -0.028227273809364753, -0.08125725790907767)', '(0.02233494523075105, -0.19910257687096494, -0.029852418967546306, 0.20238794860523618)', '(0.018352893693331748, -0.003566691954174861, -0.025804659995441584, -0.09956050480495887)', '(0.01828155985424825, -0.19830949402591153, -0.02779587009154076, 0.18487071901823054)', '(0.014315369973730022, -0.39302293898311563, -0.02409845571117615, 0.4686571319405804)', '(0.006454911194067709, -0.19756898159498013, -0.014725313072364542, 0.16847706178496963)', '(0.002503531562168106, -0.002239384993479143, -0.01135577183666515, -0.12881465358403982)', '(0.002458743862298523, -0.19719683618955125, -0.013932064908345946, 0.1602641429040782)', '(-0.0014851928614925017, -0.0018782275813918892, -0.010726782050264382, -0.13678123118148555)', '(-0.0015227574131203394, -0.19684490721773393, -0.013462406673894093, 0.1524983497771646)', '(-0.005459655557475018, -0.391771531779564, -0.010412439678350802, 0.4409039631620726)', '(-0.013295086193066298, -0.19650378548607067, -0.0015943604151093492, 0.14495701966470115)', '(-0.017225161902787712, -0.3916028676790157, 0.0013047799781846737, 0.4371365292365197)', '(-0.025057219256368026, -0.19649940994952575, 0.010047510562915068, 0.14486519696251787)', '(-0.02898720745535854, -0.0015227795257265475, 0.012944814502165426, -0.1446310678642465)', '(-0.029017663045873072, 0.19341141904615405, 0.010052193144880496, -0.43320219830460654)', '(-0.02514943466494999, -0.0018514015708651632, 0.0013881491787883643, -0.13736747022207202)', '(-0.025186462696367293, 0.19325063963002584, -0.0013592002256530762, -0.4296121343308602)']</t>
+  </si>
+  <si>
+    <t>[2, 3, 5, 8, 9, 10, 11, 12, 13]</t>
+  </si>
+  <si>
+    <t>[1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>['[-0.01881685 -0.00766736  0.03277026 -0.00908009]', '(-0.018970201901006303, 0.186969673090352, 0.032588657654782506, -0.2912461466670848)', '(-0.015230808439199262, 0.38161216242753243, 0.02676373472144081, -0.573475489083104)', '(-0.007598565190648613, 0.5763488478797438, 0.015294224939778731, -0.8576083077831207)', '(0.003928411766946263, 0.38102190616652365, -0.0018579412158836826, -0.5601558348891638)', '(0.011548849890276736, 0.5761698848745367, -0.013061057913666957, -0.8534235321243873)', '(0.02307224758776747, 0.3812283797144056, -0.0301295285561547, -0.5648760573640947)', '(0.03069681518205558, 0.1865418184533283, -0.041427049703436594, -0.2818354973558184)', '(0.034427651551122145, 0.38222944569552497, -0.04706375965055296, -0.5872911639977849)', '(0.04207224046503264, 0.5779778307046264, -0.05880958293050866, -0.8944202527410718)', '(0.05363179707912517, 0.7738458706808836, -0.0766979879853301, -1.2049944447170065)', '(0.06910871449274283, 0.9698707207933478, -0.10079787687967023, -1.5206944017112907)', '(0.08850612890860979, 1.1660561063746218, -0.13121176491389605, -1.8430632006154253)', '(0.11182725103610222, 1.362358833363228, -0.16807302892620457, -2.1734518497879227)', '(0.13907442770336678, 1.1692266578683066, -0.21154206592196304, -1.9370168960968093)']</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14]</t>
+  </si>
+  <si>
+    <t>[2, 3, 4, 5, 6, 8, 9, 11]</t>
+  </si>
+  <si>
+    <t>[1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>['[-0.01881685 -0.00766736  0.03277026 -0.00908009]', '(-0.018970201901006303, 0.186969673090352, 0.032588657654782506, -0.2912461466670848)', '(-0.015230808439199262, 0.38161216242753243, 0.02676373472144081, -0.573475489083104)', '(-0.007598565190648613, 0.5763488478797438, 0.015294224939778731, -0.8576083077831207)', '(0.003928411766946263, 0.7712591299787576, -0.0018579412158836826, -1.1454432106795691)', '(0.019353594366521412, 0.9664052992065291, -0.024766805429475063, -1.4387081936991148)', '(0.03868170035065199, 1.1618235194733544, -0.053540969303457364, -1.7390263237460089)', '(0.061918170740119086, 0.9673508153748098, -0.08832149577837754, -1.4634688048927638)', '(0.08126518704761529, 1.1634369092515942, -0.11759087187623282, -1.7823842601131068)', '(0.10453392523264718, 1.3596685305375775, -0.15323855707849496, -2.1091910721001104)', '(0.13172729584339873, 1.1663770403066074, -0.19542237852049715, -1.8675273649065207)', '(0.15505483664953087, 1.3630275465814514, -0.23277292581862757, -2.2139776607818105)']</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11]</t>
+  </si>
+  <si>
+    <t>[2, 3, 4, 5, 6, 7, 8, 9, 10]</t>
+  </si>
+  <si>
+    <t>[1, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>['[-0.01881685 -0.00766736  0.03277026 -0.00908009]', '(-0.018970201901006303, 0.186969673090352, 0.032588657654782506, -0.2912461466670848)', '(-0.015230808439199262, 0.38161216242753243, 0.02676373472144081, -0.573475489083104)', '(-0.007598565190648613, 0.5763488478797438, 0.015294224939778731, -0.8576083077831207)', '(0.003928411766946263, 0.7712591299787576, -0.0018579412158836826, -1.1454432106795691)', '(0.019353594366521412, 0.9664052992065291, -0.024766805429475063, -1.4387081936991148)', '(0.03868170035065199, 1.1618235194733544, -0.053540969303457364, -1.7390263237460089)', '(0.061918170740119086, 1.3575129579881862, -0.08832149577837754, -2.0478733797253734)', '(0.08906842989988281, 1.5534225629803073, -0.12927896337288503, -2.3665251334985395)', '(0.12013688115948895, 1.7494352078482025, -0.17660946604285582, -2.6959927759770563)', '(0.15512558531645299, 1.9453493043909325, -0.23052932156239694, -3.0369464494455816)']</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10]</t>
   </si>
   <si>
     <t>['[0,0]', '[1,1]', '[1,0]']</t>
   </si>
   <si>
-    <t>[1, 2, 3, 4, 6, 7, 8, 9]</t>
-  </si>
-  <si>
-    <t>[1, 1, 1, 1, 1, 1, 1, 1, 1, 1]</t>
-  </si>
-  <si>
-    <t>['[-0.01881685 -0.00766736  0.03277026 -0.00908009]', '(-0.018970201901006303, -0.203243578415405, 0.032588657654782506, 0.29375947416390885)', '(-0.023035073469314403, -0.3988146324758434, 0.03846384713806068, 0.5965396632322811)', '(-0.03101136611883127, -0.5944531488919764, 0.0503946404027063, 0.9010859668635411)', '(-0.0429004290966708, -0.7902203588335466, 0.06841635973997713, 1.209173733871254)', '(-0.058704836273341734, -0.5960454243559449, 0.09259983441740222, 0.9386914580939902)', '(-0.07062574476046063, -0.7922855510514539, 0.11137366357928202, 1.2589759812869332)', '(-0.08647145578148971, -0.9886422388918867, 0.1365531832050207, 1.5843623866357988)', '(-0.10624430055932745, -1.1850985480310545, 0.16824043093773666, 1.9163256445881882)', '(-0.12994627151994853, -1.3815850038887512, 0.20656694382950042, 2.2561236968378333)', '(-0.15757797159772355, -1.188916488193607, 0.2516894177662571, 2.0335645964112166)']</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10]</t>
-  </si>
-  <si>
-    <t>['[1,1]', '[1,0]', '[0,0]']</t>
-  </si>
-  <si>
-    <t>[1, 2, 3, 4, 5, 6, 7, 8, 9]</t>
-  </si>
-  <si>
-    <t>[1, 1, 1, 1, 1, 1, 1, 1, 1]</t>
-  </si>
-  <si>
-    <t>['[-0.01881685 -0.00766736  0.03277026 -0.00908009]', '(-0.018970201901006303, -0.203243578415405, 0.032588657654782506, 0.29375947416390885)', '(-0.023035073469314403, -0.3988146324758434, 0.03846384713806068, 0.5965396632322811)', '(-0.03101136611883127, -0.5944531488919764, 0.0503946404027063, 0.9010859668635411)', '(-0.0429004290966708, -0.7902203588335466, 0.06841635973997713, 1.209173733871254)', '(-0.058704836273341734, -0.9861559232896362, 0.09259983441740222, 1.5224882192013063)', '(-0.07842795473913446, -1.182266511478129, 0.12304959880142835, 1.8425792671068442)', '(-0.10207328496869704, -1.3785125418350686, 0.15990118414356524, 2.1708079305885084)', '(-0.12964353580539842, -1.5747927147279073, 0.20331734275533542, 2.508283148799749)', '(-0.16113939009995656, -1.770926329198504, 0.2534830057313304, 2.8557879869215794)']</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9]</t>
-  </si>
-  <si>
-    <t>[1,1]</t>
-  </si>
-  <si>
-    <t>[4, 22, 23, 25, 30, 42, 43]</t>
-  </si>
-  <si>
-    <t>[1, 0, 1, 0, 0, 0, 1, 0, 1, 0, 1, 0, 1, 0, 1, 0, 0, 1, 0, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 1, 1, 0, 1, 0, 1, 1, 0, 0, 0, 0, 0, 0, 1, 1]</t>
-  </si>
-  <si>
-    <t>['[-0.01881685 -0.00766736  0.03277026 -0.00908009]', '(-0.018970201901006303, 0.186969673090352, 0.032588657654782506, -0.2912461466670848)', '(-0.015230808439199262, -0.008601427704964998, 0.02676373472144081, 0.011534112466383584)', '(-0.015402836993298563, 0.18612667547570355, 0.026994416970768483, -0.27258583743663833)', '(-0.011680303483784491, 0.3808532517211452, 0.021542700222035718, -0.5566338907814913)', '(-0.004063238449361587, 0.1854355886462096, 0.010410022406405891, -0.25724234778407434)', '(-0.0003545266764373952, -0.00983342637637502, 0.005265175450724404, 0.03870579543563807)', '(-0.0005511952039648956, 0.1852126279766967, 0.006039291359437166, -0.2523112763622837)', '(0.003153057355569038, -0.009995037369338766, 0.0009930658321914924, 0.04227042267664122)', '(0.0029531566081822625, 0.1851126594944886, 0.0018384742857243167, -0.2500990170039908)', '(0.006655409798072035, -0.010035497623232886, -0.003163506054355499, 0.0431632351094689)', '(0.006454699845607377, 0.18513167393412924, -0.0023002413521661207, -0.25051612656525013)', '(0.010157333324289962, -0.009957353883328801, -0.0073105638834711235, 0.041440370621941724)', '(0.009958186246623386, 0.18526866210720294, -0.006481756471032289, -0.2535401147409823)', '(0.013663559488767445, -0.009760140805028628, -0.011552558765851935, 0.03709132125676301)', '(0.013468356672666873, 0.1855255537923259, -0.010810732340716675, -0.2592140502270008)', '(0.01717886774851339, -0.009440409240812048, -0.01599501334525669, 0.030039511553866804)', '(0.01699005956369715, -0.20432937374884574, -0.015394223114179354, 0.31763323034294655)', '(0.012903472088720235, -0.008991583835146671, -0.009041558507320423, 0.020135540619211467)', '(0.012723640412017302, -0.20398271017237296, -0.008638847694936194, 0.30995209286202646)', '(0.008643986208569841, -0.00873874722690704, -0.0024398058376956643, 0.01455728699169384)', '(0.0084692112640317, 0.1864181087331489, -0.0021486600978617874, -0.2788944278777489)', '(0.012197573438694678, 0.38157064581267675, -0.007726548655416765, -0.572254263353577)', '(0.019828986354948213, 0.5768000813278547, -0.019171633922488305, -0.8673612580395984)', '(0.031364987981505305, 0.3819441813703708, -0.03651885908328027, -0.580767236246726)', '(0.03900387160891272, 0.5775583065563445, -0.048134203808214794, -0.8847269468551164)', '(0.05055503774003961, 0.3831217982278978, -0.06582874274531712, -0.6075559787873106)', '(0.05821747370459757, 0.18897898315452172, -0.07797986232106334, -0.33631218108031996)', '(0.061997053367688, -0.004951634116738185, -0.08470610594266974, -0.06920310716765554)', '(0.06189802068535324, -0.19876346387562163, -0.08609016808602285, 0.19559846818709037)', '(0.057922751407840804, -0.0025223146077997527, -0.08217819872228105, -0.12295235193193021)', '(0.05787230511568481, -0.19637664386544298, -0.08463724576091965, 0.14271462735560358)', '(0.053944772238375946, -0.39019089486515374, -0.08178295321380757, 0.40754168694419923)', '(0.04614095434107287, -0.584063749196867, -0.0736321194749236, 0.6733615843609324)', '(0.03445967935713553, -0.7780892303849938, -0.06016488778770495, 0.9419829160554352)', '(0.018897894749435654, -0.5822103788325647, -0.041325229466596246, 0.6310184546068527)', '(0.0072536871727843615, -0.3865369242855564, -0.02870486037445919, 0.32561270211233123)', '(-0.000477051312926767, -0.5812386652299304, -0.022192606332212567, 0.6091069305860033)', '(-0.012101824617525375, -0.38581361773982537, -0.010010467720492501, 0.30951745254205715)', '(-0.019818096972321883, -0.5807915197925808, -0.0038201186696513578, 0.5990266234142377)', '(-0.0314339273681735, -0.3856163287687886, 0.008160413798633397, 0.30514286090729187)', '(-0.03914625394354927, -0.19061161349768155, 0.014263271016779235, 0.015044662343014548)', '(-0.0429584862135029, 0.004302911148992561, 0.014564164263639526, -0.27310412544596124)', '(-0.04287242799052305, 0.19921405529922126, 0.009102081754720302, -0.5611581216332401)', '(-0.03888814688453862, 0.003965553973271169, -0.0021210806779445, -0.26562152641994435)', '(-0.038808835805073195, -0.19112605971590896, -0.007433511206343387, 0.026391638576923948)', '(-0.04263135699939138, -0.38614062401615024, -0.006905678434804908, 0.31671997094390536)', '(-0.050354169479714384, -0.5811635361668052, -0.0005712790159268007, 0.607217110627252)', '(-0.06197744020305049, -0.38603360213193166, 0.01157306319661824, 0.31435430131530584)', '(-0.06969811224568911, -0.1910784055501902, 0.01786014922292436, 0.025343494461066263)']</t>
-  </si>
-  <si>
-    <t>[4, 8, 9, 10, 12, 13, 15]</t>
-  </si>
-  <si>
-    <t>[1, 0, 1, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>['[-0.01881685 -0.00766736  0.03277026 -0.00908009]', '(-0.018970201901006303, 0.186969673090352, 0.032588657654782506, -0.2912461466670848)', '(-0.015230808439199262, -0.008601427704964998, 0.02676373472144081, 0.011534112466383584)', '(-0.015402836993298563, 0.18612667547570355, 0.026994416970768483, -0.27258583743663833)', '(-0.011680303483784491, 0.3808532517211452, 0.021542700222035718, -0.5566338907814913)', '(-0.004063238449361587, 0.1854355886462096, 0.010410022406405891, -0.25724234778407434)', '(-0.0003545266764373952, -0.00983342637637502, 0.005265175450724404, 0.03870579543563807)', '(-0.0005511952039648956, 0.1852126279766967, 0.006039291359437166, -0.2523112763622837)', '(0.003153057355569038, 0.3802478236181868, 0.0009930658321914924, -0.5430831938294477)', '(0.010758013827932775, 0.5753558045012619, -0.009868598044397462, -0.835453059538741)', '(0.022265129917958013, 0.7706111653268025, -0.02657765923517228, -1.1312231597978708)', '(0.037677353224494066, 0.5758470842321526, -0.0492021224311297, -0.8469931259337694)', '(0.04919429490913712, 0.7716044573942316, -0.06614198494980508, -1.1547334213814318)', '(0.06462638405702176, 0.9675236136254655, -0.08923665337743372, -1.4674011335183674)', '(0.08397685632953107, 0.7736001424636361, -0.11858467604780107, -1.203874114267977)', '(0.09944885917880379, 0.9700384112626529, -0.1426621583331606, -1.5312444009815376)', '(0.11884962740405686, 0.7768952435383929, -0.17328704635279135, -1.2862734072748148)', '(0.13438753227482472, 0.5843495601660582, -0.19901251449828766, -1.0524722220904958)', '(0.1460745234781459, 0.3923424507252501, -0.22006195894009759, -0.828270452067901)']</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18]</t>
-  </si>
-  <si>
-    <t>[2, 3, 11, 12, 14, 18, 19, 20, 21, 22, 23, 26]</t>
-  </si>
-  <si>
-    <t>[1, 0, 0, 0, 0, 0, 0, 1, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>['[-0.01881685 -0.00766736  0.03277026 -0.00908009]', '(-0.018970201901006303, 0.186969673090352, 0.032588657654782506, -0.2912461466670848)', '(-0.015230808439199262, 0.38161216242753243, 0.02676373472144081, -0.573475489083104)', '(-0.007598565190648613, 0.5763488478797438, 0.015294224939778731, -0.8576083077831207)', '(0.003928411766946263, 0.38102190616652365, -0.0018579412158836826, -0.5601558348891638)', '(0.011548849890276736, 0.18592608100371844, -0.013061057913666957, -0.2680588366431443)', '(0.015267371510351105, -0.009007059353799696, -0.018422234646529843, 0.020476091983435085)', '(0.015087230323275112, -0.20386003791969498, -0.01801271280686114, 0.30729013388006127)', '(0.011010029564881212, -0.008486111063197549, -0.011866910129259915, 0.00898133406309054)', '(0.010840307343617262, -0.2034358816365489, -0.011687283447998104, 0.29789661033210013)', '(0.006771589710886284, -0.008149296488200092, -0.005729351241356101, 0.0015507552970182026)', '(0.006608603781122282, 0.18705435135362433, -0.005698336135415737, -0.2929343307904983)', '(0.010349690808194768, 0.3822570824520565, -0.011557022751225703, -0.5874089753823313)', '(0.017994832457235897, 0.18729887594746272, -0.02330520225887233, -0.29838888412220915)', '(0.021740809976185153, 0.3827451467553024, -0.029272979941316515, -0.5983297882762659)', '(0.0293957129112912, 0.18804475482900257, -0.041239575706841836, -0.31500934862805474)', '(0.03315660800787125, -0.006466230614868118, -0.04753976267940293, -0.03561193817990749)', '(0.033027283395573884, -0.2008753528123006, -0.048252001443001076, 0.2417008532760307)', '(0.029009776339327872, -0.005098546610226268, -0.04341798437748046, -0.06580314276870586)', '(0.028907805407123347, 0.19061813707107458, -0.04473404723285458, -0.3718623767054856)', '(0.03272016814854484, 0.3863461111775709, -0.05217129476696429, -0.6783080521784348)', '(0.040447090372096255, 0.5821525488449457, -0.06573745581053299, -0.9869494869063913)', '(0.05209014134899517, 0.7780902650829915, -0.08547644554866081, -1.2995341392212718)', '(0.067651946650655, 0.9741868734255439, -0.11146712833308625, -1.6177046468698166)', '(0.08713568411916589, 0.7805416357587185, -0.14382122127048258, -1.361742957102464)', '(0.10274651683434026, 0.5874848558030563, -0.17105608041253187, -1.1172854176104525)', '(0.11449621395040138, 0.784387644584122, -0.19340178876474093, -1.4583746628066627)', '(0.13018396684208383, 0.5920916658188935, -0.22256928202087417, -1.2318147360393588)']</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27]</t>
-  </si>
-  <si>
-    <t>[8, 9, 10, 11, 12, 13, 14, 15, 16]</t>
-  </si>
-  <si>
-    <t>[1, 0, 1, 0, 1, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>['[-0.01881685 -0.00766736  0.03277026 -0.00908009]', '(-0.018970201901006303, 0.186969673090352, 0.032588657654782506, -0.2912461466670848)', '(-0.015230808439199262, -0.008601427704964998, 0.02676373472144081, 0.011534112466383584)', '(-0.015402836993298563, 0.18612667547570355, 0.026994416970768483, -0.27258583743663833)', '(-0.011680303483784491, -0.009369849307344524, 0.021542700222035718, 0.028487507456279093)', '(-0.011867700469931382, 0.1854366465508055, 0.0221124503711613, -0.2573213694562454)', '(-0.008158967538915273, -0.009993906974345684, 0.01696602298203639, 0.04225332601995413)', '(-0.008358845678402187, 0.1848806988513335, 0.017811089502435474, -0.2450287418665169)', '(-0.004661231701375517, 0.3797437874814581, 0.012910514665105136, -0.532040829553236)', '(0.002933644048253645, 0.5746817915426519, 0.0022696980740404167, -0.8206278807133297)', '(0.014427279879106683, 0.769772609746117, -0.014142859540226177, -1.112596063595955)', '(0.029822732074029024, 0.9650774255497784, -0.03639478081214528, -1.4096818511601423)', '(0.04912428058502459, 1.160631381333048, -0.06458841783534813, -1.7135162396565267)', '(0.07233690821168555, 1.3564324805121815, -0.09885874262847866, -2.0255812840875524)', '(0.09946555782192917, 1.5524282125649003, -0.1393703683102297, -2.3471565966113146)', '(0.13051412207322718, 1.7484996227530742, -0.186313500242456, -2.679254316514289)', '(0.16548411452828868, 1.9444429424972856, -0.23989858657274177, -3.022542555141353)']</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16]</t>
-  </si>
-  <si>
-    <t>['[1,0]', '[0,0]', '[1,1]']</t>
-  </si>
-  <si>
-    <t>[2, 3, 4, 5, 6, 7, 8, 9, 10]</t>
-  </si>
-  <si>
-    <t>[1, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>['[-0.01881685 -0.00766736  0.03277026 -0.00908009]', '(-0.018970201901006303, 0.186969673090352, 0.032588657654782506, -0.2912461466670848)', '(-0.015230808439199262, 0.38161216242753243, 0.02676373472144081, -0.573475489083104)', '(-0.007598565190648613, 0.5763488478797438, 0.015294224939778731, -0.8576083077831207)', '(0.003928411766946263, 0.7712591299787576, -0.0018579412158836826, -1.1454432106795691)', '(0.019353594366521412, 0.9664052992065291, -0.024766805429475063, -1.4387081936991148)', '(0.03868170035065199, 1.1618235194733544, -0.053540969303457364, -1.7390263237460089)', '(0.061918170740119086, 1.3575129579881862, -0.08832149577837754, -2.0478733797253734)', '(0.08906842989988281, 1.5534225629803073, -0.12927896337288503, -2.3665251334985395)', '(0.12013688115948895, 1.7494352078482025, -0.17660946604285582, -2.6959927759770563)', '(0.15512558531645299, 1.9453493043909325, -0.23052932156239694, -3.0369464494455816)']</t>
-  </si>
-  <si>
     <t>[1,0]</t>
   </si>
   <si>
-    <t>[3, 7, 10, 19, 28, 30, 35, 39, 43, 45, 48]</t>
-  </si>
-  <si>
-    <t>[1, 0, 1, 1, 1, 0, 1, 1, 1, 1, 1, 1, 0, 1, 0, 1, 0, 0, 1, 1, 1, 1, 0, 1, 0, 0, 1, 0, 0, 0, 0, 0, 0, 1, 0, 0, 0, 1, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>['[-0.01881685 -0.00766736  0.03277026 -0.00908009]', '(-0.018970201901006303, 0.186969673090352, 0.032588657654782506, -0.2912461466670848)', '(-0.015230808439199262, -0.008601427704964998, 0.02676373472144081, 0.011534112466383584)', '(-0.015402836993298563, -0.20409677944981686, 0.026994416970768483, 0.3125397204020826)', '(-0.0194847725822949, -0.009369587627564041, 0.03324521137881013, 0.028490744028419945)', '(-0.01967216433484618, 0.18526022195347203, 0.03381502625937853, -0.2535203583332872)', '(-0.01596695989577674, -0.010327838532409511, 0.028744619092712788, 0.04963373681676758)', '(-0.01617351666642493, -0.20584991601057387, 0.02973729382904814, 0.3512454526255887)', '(-0.020290514986636407, -0.011163204504964663, 0.036762202881559916, 0.06808597381183934)', '(-0.0205137790767357, 0.18341293159795002, 0.0381239223577967, -0.21277537785557532)', '(-0.0168455204447767, -0.012232762736956448, 0.03386841480068519, 0.09168563923012446)', '(-0.01709017569951583, 0.18238778628259583, 0.03570212758528768, -0.19012235738965755)', '(-0.013442419973863914, 0.37698126915451957, 0.031899680437494526, -0.4713323779112896)', '(-0.005902794590773522, 0.18142360860968812, 0.02247303287926873, -0.168768206970143)', '(-0.00227432241857976, 0.3762167994174709, 0.01909766873986587, -0.454277697385924)', '(0.005250013569769658, 0.18083008469507156, 0.010012114792147392, -0.15563669658421114)', '(0.00886661526367109, 0.37580726366098777, 0.0068993808604631696, -0.44514429384319815)', '(0.016382760536890844, 0.1805883820870695, -0.002003505016400793, -0.15029453910155688)', '(0.019994528178632235, -0.014504822866986289, -0.005009395798431931, 0.14175565091613884)', '(0.01970443172129251, -0.20955467329060173, -0.0021742827801091535, 0.4328539994116084)', '(0.015513338255480475, -0.01440200472140929, 0.006482797208123014, 0.13948644986286396)', '(0.01522529816105229, 0.18062649963114075, 0.009272526205380292, -0.15114423036090968)', '(0.018837828153675105, 0.375614456861941, 0.006249641598162098, -0.4408875088971466)', '(0.026350117290913924, 0.1804046220327518, -0.002568108579780834, -0.14624109234794036)', '(0.02995820973156896, 0.3755632557641364, -0.005492930426739641, -0.4397331007080996)', '(0.03746947484685169, 0.1805194739896365, -0.014287592440901633, -0.1487867551471277)', '(0.04107986432664442, -0.014394997510093266, -0.017263327543844187, 0.13935470165176234)', '(0.04079196437644256, 0.18096989904083655, -0.01447623351080894, -0.1587241431147115)', '(0.04441136235725929, 0.3762960809580329, -0.01765071637310317, -0.4559385809192499)', '(0.051937283976419946, 0.181428076502003, -0.026769487991488167, -0.16887114723979924)', '(0.05556584550646001, 0.3769227650539323, -0.030146910936284153, -0.46987740644530684)', '(0.06310430080753865, 0.18223935265710936, -0.03954445906519029, -0.18684682864990848)', '(0.06674908786068083, -0.012295163356420308, -0.04328139563818846, 0.09310377938067904)', '(0.06650318459355242, -0.206770896837105, -0.04141932005057488, 0.37182343388014755)', '(0.06236776665681032, -0.011085746241844552, -0.033982851372971926, 0.06637365563292047)', '(0.06214605173197343, 0.18450652643910823, -0.03265537826031352, -0.23683439763986058)', '(0.06583618226075559, -0.01013403651358566, -0.03739206621311073, 0.045371815954477535)', '(0.06563350153048388, -0.20470040976200082, -0.03648462989402118, 0.3260266665331402)', '(0.06153949333524386, -0.009078507465461239, -0.029964096563358376, 0.02206498817416508)', '(0.06135792318593464, 0.18646005906121052, -0.029522796799875076, -0.2799193248618755)', '(0.06508712436715886, -0.008228581816473263, -0.035121183297112585, 0.0033079369370452305)', '(0.06492255273082939, -0.20282970166109585, -0.03505502455837168, 0.2847060999627393)', '(0.060865958697607477, -0.0072257742131757174, -0.029360902559116893, -0.018823599609198716)', '(0.06072144321334396, 0.18830467313530927, -0.029737374551300867, -0.32062372526921046)', '(0.06448753667605014, -0.006381440394251703, -0.03614984905668508, -0.037465167445719094)', '(0.06435990786816512, 0.18923975429523415, -0.03689915240559946, -0.34133099128861105)', '(0.0681447029540698, -0.005338306365177348, -0.04372577223137168, -0.060508462418498055)', '(0.06803793682676625, -0.19980693267084904, -0.04493594147974164, 0.2180643807787293)', '(0.06404179817334926, -0.004072385607001128, -0.04057465386416706, -0.08844778475434029)', '(0.06396035046120924, -0.19858996598916945, -0.04234360955925386, 0.19116276728201576)']</t>
-  </si>
-  <si>
-    <t>[1, 3, 4, 5, 10, 11, 14, 19, 22, 24, 30, 32, 34, 35]</t>
-  </si>
-  <si>
-    <t>[1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 1, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0]</t>
-  </si>
-  <si>
-    <t>['[-0.01881685 -0.00766736  0.03277026 -0.00908009]', '(-0.018970201901006303, -0.203243578415405, 0.032588657654782506, 0.29375947416390885)', '(-0.023035073469314403, -0.008601042343346021, 0.03846384713806068, 0.01153006168279358)', '(-0.023207094316181322, -0.20425290291665268, 0.03869444837171655, 0.31609636674495395)', '(-0.027292152374514374, -0.39990404041704386, 0.04501637570661563, 0.6207267240778034)', '(-0.03529023318285525, -0.5956248027752826, 0.0574309101881717, 0.9272407954660062)', '(-0.0472027292383609, -0.4013233792000955, 0.07597572609749183, 0.6531445849773836)', '(-0.05522919682236281, -0.20733702810799612, 0.0890386177970395, 0.3853198470539871)', '(-0.05937593738452274, -0.013584499374372339, 0.09674501473811925, 0.12198510636795673)', '(-0.05964762737201018, 0.180027848286615, 0.09918471686547839, -0.13867668869199345)', '(-0.056047070406277884, -0.01636448321923309, 0.09641118309163851, 0.183576491992188)', '(-0.056374360070662544, -0.21272425778850657, 0.10008271293148227, 0.5050493203835824)', '(-0.06062884522643268, -0.019144614200988758, 0.11018369933915392, 0.24550811208692463)', '(-0.061011737510452455, 0.17424526712264163, 0.11509386158089241, -0.010489109786070427)', '(-0.05752683216799962, -0.0223230614077993, 0.114884079385171, 0.31617558102843096)', '(-0.05797329339615561, 0.170991052824173, 0.12120759100573962, 0.061817547302318865)', '(-0.05455347233967215, 0.36418547231108345, 0.122443941951786, -0.1903001399805469)', '(-0.04726976289345048, 0.5573623516934195, 0.11863793915217506, -0.4419873805976633)', '(-0.03612251585958209, 0.750623236961458, 0.1097981915402218, -0.6950432054516658)', '(-0.021110051120352927, 0.5541634943191229, 0.09589732743118848, -0.36991229730609393)', '(-0.010026781233970468, 0.7478014363138215, 0.0884990814850666, -0.6308840484130958)', '(0.004929247492305961, 0.941584354409572, 0.07588140051680468, -0.8944360949707723)', '(0.0237609345804974, 0.745519941012692, 0.05799267861738924, -0.5788980422945773)', '(0.03867133340075124, 0.9397832543241489, 0.04641471777149769, -0.8527628547140089)', '(0.05746699848723422, 0.7440603520251098, 0.029359460677217515, -0.5458536547796053)', '(0.07234820552773641, 0.9387577444396384, 0.01844238758162541, -0.8291434423614261)', '(0.09112336041652919, 1.1336227845664935, 0.0018595187343968846, -1.1159695410008432)', '(0.11379581610785905, 0.9384764739001382, -0.02045987208561998, -0.8227038828924523)', '(0.1325653455858618, 0.7436403228618333, -0.036913949743469024, -0.5365256066759703)', '(0.14743815204309846, 0.9392613332352104, -0.047644461876988425, -0.8406074608948697)', '(0.16622337870780268, 1.1350002220903925, -0.06445661109488582, -1.1478847854363794)', '(0.18892338314961055, 0.940776275197653, -0.08741430680361341, -0.8760909801048395)', '(0.2077389086535636, 1.136970708673348, -0.1049361264057102, -1.1949260553311114)', '(0.23047832282703057, 0.9433521929846349, -0.12883464751233242, -0.9368904830426873)', '(0.24934536668672327, 1.1399539629643476, -0.14757245717318618, -1.267121759794398)', '(0.2721444459460102, 1.3366202845622102, -0.17291489236907415, -1.60214387130504)', '(0.2988768516372544, 1.1439155897067512, -0.20495776979517494, -1.367981434693699)', '(0.32175516343138943, 0.9518619222820315, -0.23231739848904892, -1.1457671685948965)']</t>
-  </si>
-  <si>
-    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37]</t>
-  </si>
-  <si>
-    <t>[1, 2, 3, 4, 5, 6, 8]</t>
-  </si>
-  <si>
-    <t>['[-0.01881685 -0.00766736  0.03277026 -0.00908009]', '(-0.018970201901006303, -0.203243578415405, 0.032588657654782506, 0.29375947416390885)', '(-0.023035073469314403, -0.3988146324758434, 0.03846384713806068, 0.5965396632322811)', '(-0.03101136611883127, -0.5944531488919764, 0.0503946404027063, 0.9010859668635411)', '(-0.0429004290966708, -0.7902203588335466, 0.06841635973997713, 1.209173733871254)', '(-0.058704836273341734, -0.9861559232896362, 0.09259983441740222, 1.5224882192013063)', '(-0.07842795473913446, -1.182266511478129, 0.12304959880142835, 1.8425792671068442)', '(-0.10207328496869704, -0.9886983365154707, 0.15990118414356524, 1.5905077322082546)', '(-0.12184725169900645, -1.1853169349858783, 0.19171133878773033, 1.9284841128542352)', '(-0.145553590398724, -0.992697878202941, 0.23028102104481504, 1.7008673290687473)']</t>
-  </si>
-  <si>
-    <t>[1, 2, 4, 5, 6, 7, 8, 9, 10]</t>
-  </si>
-  <si>
-    <t>['[-0.01881685 -0.00766736  0.03277026 -0.00908009]', '(-0.018970201901006303, -0.203243578415405, 0.032588657654782506, 0.29375947416390885)', '(-0.023035073469314403, -0.3988146324758434, 0.03846384713806068, 0.5965396632322811)', '(-0.03101136611883127, -0.2042514664103063, 0.0503946404027063, 0.31621635780497453)', '(-0.035096395447037396, -0.40005365906793083, 0.056718967558805795, 0.6243565322687714)', '(-0.043097468628396016, -0.595919684308709, 0.06920609820418122, 0.9343495519973364)', '(-0.055015862314570195, -0.791903516316987, 0.08789308924412795, 1.2479519400188712)', '(-0.07085393264090993, -0.9880355484185881, 0.11285212804450537, 1.5668216613877721)', '(-0.09061464360928169, -1.184310416098135, 0.14418856127226082, 1.892469338400986)', '(-0.1143008519312444, -1.3806729853307276, 0.18203794804028053, 2.2262013605705073)', '(-0.14191431163785895, -1.5770022075612058, 0.2265619752516907, 2.5690532739686676)']</t>
+    <t>[4, 10, 13, 19, 27, 29, 31, 39, 40, 41, 42]</t>
+  </si>
+  <si>
+    <t>[1, 0, 1, 0, 0, 0, 1, 0, 1, 0, 0, 0, 0, 0, 0, 1, 0, 1, 0, 0, 0, 1, 0, 1, 0, 1, 0, 0, 0, 0, 0, 0, 0, 1, 0, 1, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>['[-0.01881685 -0.00766736  0.03277026 -0.00908009]', '(-0.018970201901006303, 0.186969673090352, 0.032588657654782506, -0.2912461466670848)', '(-0.015230808439199262, -0.008601427704964998, 0.02676373472144081, 0.011534112466383584)', '(-0.015402836993298563, 0.18612667547570355, 0.026994416970768483, -0.27258583743663833)', '(-0.011680303483784491, 0.3808532517211452, 0.021542700222035718, -0.5566338907814913)', '(-0.004063238449361587, 0.1854355886462096, 0.010410022406405891, -0.25724234778407434)', '(-0.0003545266764373952, -0.00983342637637502, 0.005265175450724404, 0.03870579543563807)', '(-0.0005511952039648956, 0.1852126279766967, 0.006039291359437166, -0.2523112763622837)', '(0.003153057355569038, -0.009995037369338766, 0.0009930658321914924, 0.04227042267664122)', '(0.0029531566081822625, 0.1851126594944886, 0.0018384742857243167, -0.2500990170039908)', '(0.006655409798072035, 0.3802083083022956, -0.003163506054355499, -0.5422014845146548)', '(0.014259575964117945, 0.185130961605942, -0.014007535744648594, -0.25051699791455684)', '(0.017962195196236784, -0.009788186702095414, -0.01901787570293973, 0.0377149602103119)', '(0.017766431462194875, 0.18560124630373379, -0.018263576498733492, -0.26090710803969486)', '(0.021478456388269552, -0.009255294323694818, -0.02348171865952739, 0.025959764265578222)', '(0.021293350501795656, -0.2040327655620164, -0.022962523374215824, 0.3111424350289726)', '(0.01721269519055533, -0.008591321540890401, -0.016739674673636372, 0.011307165891101922)', '(0.01704086875973752, -0.2034692529239597, -0.016513531355814334, 0.2986618733715765)', '(0.012971483701258326, -0.008115851162209725, -0.010540293888382804, 0.0008169664291077239)', '(0.012809166678014131, 0.18715566476967552, -0.010523954559800649, -0.29517282596752015)', '(0.016552279973407642, -0.007814683257940463, -0.016427411079151053, -0.005827484558599549)', '(0.016395986308248834, -0.20269723651527682, -0.016543960770323045, 0.28162746134581595)', '(0.012342041577943297, -0.007343256085819316, -0.010911411543406725, -0.01622711112953884)', '(0.01219517645622691, -0.20230703853496365, -0.011235953765997501, 0.2729932622483135)', '(0.008149035685527637, -0.007026581618968797, -0.005776088521031232, -0.02321223409261597)', '(0.008008504053148261, -0.20206522403010435, -0.006240333202883551, 0.2676426886204662)', '(0.003967199572546175, -0.006854771954307781, -0.0008874794304742266, -0.027001934187224963)', '(0.003830104133460019, 0.18827989513527466, -0.0014275181142187259, -0.31996473847097806)', '(0.007595702036165513, -0.0068216969031378305, -0.007826812883638288, -0.027732338781031485)', '(0.007459268098102756, 0.1884116167210654, -0.008381459659258917, -0.3228743989091573)', '(0.011227500432524063, -0.006589987842972045, -0.014838947637442063, -0.03284638627346076)', '(0.011095700675664621, 0.18874158183519782, -0.015495875362911278, -0.33017397370111967)', '(0.014870532312368578, -0.006156395374572798, -0.02209935483693367, -0.04241771171022779)', '(0.014747404404877122, -0.200954591450201, -0.022947709071138224, 0.24321155195088556)', '(0.010728312575873103, -0.005512505558905562, -0.018083478032120515, -0.0566204251662607)', '(0.010618062464694992, -0.20037056433044706, -0.019215886535445727, 0.23030262079094932)', '(0.006610651178086051, -0.0049793697802490156, -0.014609834119626741, -0.06837918447687658)', '(0.0065110637824810705, -0.19988884715757047, -0.01597741780916427, 0.2196586915449233)', '(0.0025132868393296613, -0.004542195998140708, -0.011584243978265806, -0.07802104621369854)', '(0.0024224429193668473, 0.19074388912217685, -0.013144664902539778, -0.3743362109019673)', '(0.006237320701810384, 0.3860500663693485, -0.020631389120579123, -0.6711345882569026)', '(0.013958322029197355, 0.581452667384027, -0.034054080885717174, -0.970241309636297)', '(0.025587375376877896, 0.7770147690269834, -0.05345890707844311, -1.2734243511738559)', '(0.041127670757417564, 0.5826141147447862, -0.07892739410192023, -0.9979493807898524)', '(0.05277995305231329, 0.3886310333273995, -0.09888638171771728, -0.7310611753578937)', '(0.06055257371886128, 0.19500464257024896, -0.11350760522487516, -0.4710657048299657)', '(0.06445266657026626, 0.0016535860132194102, -0.12292891932147447, -0.21620508576848763)', '(0.06448573829053064, -0.19151616578711797, -0.12725302103684422, 0.03531283468608715)', '(0.06065541497478828, -0.3846053601341124, -0.12654676434312248, 0.2852932230171201)', '(0.05296330777210603, -0.5777167058533009, -0.12084089988278007, 0.5355384310425901)']</t>
+  </si>
+  <si>
+    <t>[3, 9, 12, 13, 14, 18, 21, 24, 27, 29, 31, 32, 34, 35]</t>
+  </si>
+  <si>
+    <t>[1, 0, 1, 1, 1, 0, 1, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>['[-0.01881685 -0.00766736  0.03277026 -0.00908009]', '(-0.018970201901006303, 0.186969673090352, 0.032588657654782506, -0.2912461466670848)', '(-0.015230808439199262, -0.008601427704964998, 0.02676373472144081, 0.011534112466383584)', '(-0.015402836993298563, -0.20409677944981686, 0.026994416970768483, 0.3125397204020826)', '(-0.0194847725822949, -0.009369587627564041, 0.03324521137881013, 0.028490744028419945)', '(-0.01967216433484618, 0.18526022195347203, 0.03381502625937853, -0.2535203583332872)', '(-0.01596695989577674, -0.010327838532409511, 0.028744619092712788, 0.04963373681676758)', '(-0.01617351666642493, 0.18437040116260206, 0.02973729382904814, -0.2338432242158895)', '(-0.01248610864317289, 0.3790551202362022, 0.02506042934473035, -0.5169997157029684)', '(-0.004905006238448845, 0.5738154050360953, 0.014720435030670982, -0.8016814168792781)', '(0.006571301862273061, 0.37849469804643954, -0.0013131933069145795, -0.5044044474304192)', '(0.014141195823201853, 0.18339127857878582, -0.011401282255522964, -0.21213564928864137)', '(0.01780902139477757, 0.3786743688143266, -0.01564399524129579, -0.5083931506866917)', '(0.0253825087710641, 0.5740131988659343, -0.025811858255029622, -0.8059646888699243)', '(0.03686277274838279, 0.7694792825422476, -0.04193115203242811, -1.1066539912434619)', '(0.05225235839922774, 0.574932909377613, -0.06406423185729734, -0.827415082150899)', '(0.06375101658678001, 0.38074269814595313, -0.08061253350031533, -0.5555493142863767)', '(0.07136587054969908, 0.18683959954623294, -0.09172351978604286, -0.2893136213147877)', '(0.07510266254062374, 0.38314164976805365, -0.09750979221233862, -0.6094578358864859)', '(0.08276549553598482, 0.1895082925730556, -0.10969894893006833, -0.34900999970394625)', '(0.08655566138744593, -0.003896400571691161, -0.11667914892414726, -0.09283360878297264)', '(0.08647773337601211, 0.1926878355861699, -0.1185358210998067, -0.41993089992432)', '(0.09033149008773551, -0.0005726002672226393, -0.1269344390982931, -0.16684243028810541)', '(0.09032003808239106, -0.19367062179295633, -0.13027128770405522, 0.08325569558904428)', '(0.08644662564653192, 0.0030547609092573536, -0.12860617379227432, -0.24752352756385165)', '(0.08650772086471707, -0.1900183517157828, -0.13355664434355136, 0.0019883601363474)', '(0.08270735383040141, -0.3829972247344573, -0.1335168771408244, 0.24972980240321918)', '(0.07504740933571226, -0.18624634127125234, -0.12852228109276004, -0.08190729310705203)', '(0.07132248251028721, -0.3793140981310308, -0.13016042695490107, 0.16762420311788404)', '(0.06373620054766659, -0.18259251562512036, -0.12680794289254338, -0.16312129864743072)', '(0.06008435023516418, -0.3756925845610958, -0.130070368865492, 0.08702140066684796)', '(0.052570498543942266, -0.17896931894930523, -0.12832994085215504, -0.24370379917566717)', '(0.04899111216495616, 0.017729788595907597, -0.13320401683566838, -0.5739518082754359)', '(0.04934570793687432, -0.17529789522572456, -0.1446830530011771, -0.32602147232654344)', '(0.04583975003235983, 0.0215558135181812, -0.15120348244770795, -0.6606054091924652)', '(0.04627086630272345, 0.2184223836824022, -0.16441559063155725, -0.9968206752185418)', '(0.050639313976371496, 0.025834972630352115, -0.1843520041359281, -0.7599560523727782)', '(0.05115601342897854, -0.1663333964373908, -0.19955112518338367, -0.5304808784273469)', '(0.04782934550023073, -0.3581717064554617, -0.2101607427519306, -0.30671321008101515)']</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12, 13, 14, 15, 16, 17, 18, 19, 20, 21, 22, 23, 24, 25, 26, 27, 28, 29, 30, 31, 32, 33, 34, 35, 36, 37, 38]</t>
+  </si>
+  <si>
+    <t>[2, 6, 8, 9, 10, 12, 13, 17, 18]</t>
+  </si>
+  <si>
+    <t>[1, 0, 0, 0, 1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>['[-0.01881685 -0.00766736  0.03277026 -0.00908009]', '(-0.018970201901006303, 0.186969673090352, 0.032588657654782506, -0.2912461466670848)', '(-0.015230808439199262, 0.38161216242753243, 0.02676373472144081, -0.573475489083104)', '(-0.007598565190648613, 0.1861253929542234, 0.015294224939778731, -0.27248274994439964)', '(-0.003876057331564145, -0.009211414773523385, 0.009844569940890738, 0.024984520240536767)', '(-0.004060285627034613, 0.18576798339470538, 0.010344260345701474, -0.26457614791114553)', '(-0.00034492595914050513, 0.38074077330267914, 0.005052737387478563, -0.5539785274968766)', '(0.007269889506913077, 0.18554823711507773, -0.006026833162458969, -0.25970796220825093)', '(0.010980854249214632, 0.380755704458433, -0.011220992406623987, -0.5542857236131895)', '(0.01859596833838329, 0.576033405308437, -0.022306706878887778, -0.8504827369606776)', '(0.030116636444552033, 0.77145230734941, -0.03931636161810133, -1.1500957922556303)', '(0.04554568259154023, 0.5768649039161928, -0.06231827746321393, -0.8699962820990513)', '(0.057082980669864086, 0.7727766912853318, -0.07971820310519495, -1.18160323731488)', '(0.07253851449557072, 0.9688376336062623, -0.10335026785149255, -1.4981730070778825)', '(0.09191526716769596, 0.7751123021154007, -0.1333137279930502, -1.2394664704216047)', '(0.10741751321000398, 0.5819302071032892, -0.15810305740148228, -0.9913427625385114)', '(0.11905611735206977, 0.38923664436578564, -0.1779299126522525, -0.7521963002781853)', '(0.1268408502393855, 0.5863074329735648, -0.1929738386578162, -1.0951713187210455)', '(0.1385669988988568, 0.7833739719614693, -0.2148772650322371, -1.4416671228084583)']</t>
+  </si>
+  <si>
+    <t>[2, 4, 5, 6, 7, 8, 9, 10, 11, 12]</t>
+  </si>
+  <si>
+    <t>[1, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0]</t>
+  </si>
+  <si>
+    <t>['[-0.01881685 -0.00766736  0.03277026 -0.00908009]', '(-0.018970201901006303, 0.186969673090352, 0.032588657654782506, -0.2912461466670848)', '(-0.015230808439199262, 0.38161216242753243, 0.02676373472144081, -0.573475489083104)', '(-0.007598565190648613, 0.1861253929542234, 0.015294224939778731, -0.27248274994439964)', '(-0.003876057331564145, 0.38102580903871064, 0.009844569940890738, -0.5603028555498686)', '(0.003744458849210068, 0.5760082163585145, -0.0013614871701066334, -0.8498680372101901)', '(0.015264623176380358, 0.7711487074207513, -0.018358847914310437, -1.142978779616701)', '(0.030687597324795382, 0.9665056771590287, -0.04121842350664446, -1.4413620502969484)', '(0.050017710867975955, 1.1621102689106992, -0.07004566451258343, -1.7466345155681449)', '(0.07325991624618994, 1.3579549924664167, -0.10497835482394632, -2.0602578163979106)', '(0.10041901609551827, 1.5539800288874153, -0.14618351115190453, -2.383483623618145)', '(0.13149861667326657, 1.7500569815548495, -0.19385318362426743, -2.7172871229411517)', '(0.16649975630436356, 1.9459702533623404, -0.24819892608309047, -3.062289173566951)']</t>
+  </si>
+  <si>
+    <t>[0, 1, 2, 3, 4, 5, 6, 7, 8, 9, 10, 11, 12]</t>
   </si>
 </sst>
 </file>
@@ -668,7 +677,7 @@
         <v>18</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G2" t="s">
         <v>19</v>
@@ -718,7 +727,7 @@
         <v>18</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G3" t="s">
         <v>19</v>
@@ -768,13 +777,13 @@
         <v>24</v>
       </c>
       <c r="F4">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="G4" t="s">
         <v>25</v>
       </c>
       <c r="H4">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="I4" t="s">
         <v>26</v>
@@ -783,10 +792,10 @@
         <v>100</v>
       </c>
       <c r="K4" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="L4">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -798,7 +807,7 @@
         <v>3</v>
       </c>
       <c r="P4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -818,13 +827,13 @@
         <v>24</v>
       </c>
       <c r="F5">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="G5" t="s">
         <v>25</v>
       </c>
       <c r="H5">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="I5" t="s">
         <v>26</v>
@@ -833,10 +842,10 @@
         <v>100</v>
       </c>
       <c r="K5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="L5">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -848,7 +857,7 @@
         <v>3</v>
       </c>
       <c r="P5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -865,40 +874,40 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6">
+        <v>7</v>
+      </c>
+      <c r="G6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6">
+        <v>18</v>
+      </c>
+      <c r="I6" t="s">
         <v>29</v>
       </c>
-      <c r="F6">
-        <v>11</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="J6">
+        <v>100</v>
+      </c>
+      <c r="K6" t="s">
         <v>30</v>
       </c>
-      <c r="H6">
-        <v>17</v>
-      </c>
-      <c r="I6" t="s">
+      <c r="L6">
+        <v>19</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6" t="s">
+        <v>22</v>
+      </c>
+      <c r="O6">
+        <v>3</v>
+      </c>
+      <c r="P6" t="s">
         <v>31</v>
-      </c>
-      <c r="J6">
-        <v>100</v>
-      </c>
-      <c r="K6" t="s">
-        <v>32</v>
-      </c>
-      <c r="L6">
-        <v>18</v>
-      </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-      <c r="N6" t="s">
-        <v>22</v>
-      </c>
-      <c r="O6">
-        <v>3</v>
-      </c>
-      <c r="P6" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -915,40 +924,40 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7">
+        <v>7</v>
+      </c>
+      <c r="G7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7">
+        <v>18</v>
+      </c>
+      <c r="I7" t="s">
         <v>29</v>
       </c>
-      <c r="F7">
-        <v>11</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="J7">
+        <v>100</v>
+      </c>
+      <c r="K7" t="s">
         <v>30</v>
       </c>
-      <c r="H7">
-        <v>17</v>
-      </c>
-      <c r="I7" t="s">
+      <c r="L7">
+        <v>19</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O7">
+        <v>3</v>
+      </c>
+      <c r="P7" t="s">
         <v>31</v>
-      </c>
-      <c r="J7">
-        <v>100</v>
-      </c>
-      <c r="K7" t="s">
-        <v>32</v>
-      </c>
-      <c r="L7">
-        <v>18</v>
-      </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-      <c r="N7" t="s">
-        <v>22</v>
-      </c>
-      <c r="O7">
-        <v>3</v>
-      </c>
-      <c r="P7" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -965,40 +974,40 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8">
+        <v>11</v>
+      </c>
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8">
+        <v>22</v>
+      </c>
+      <c r="I8" t="s">
         <v>34</v>
       </c>
-      <c r="F8">
-        <v>8</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="J8">
+        <v>100</v>
+      </c>
+      <c r="K8" t="s">
         <v>35</v>
       </c>
-      <c r="H8">
-        <v>10</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="L8">
+        <v>23</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8" t="s">
+        <v>22</v>
+      </c>
+      <c r="O8">
+        <v>3</v>
+      </c>
+      <c r="P8" t="s">
         <v>36</v>
-      </c>
-      <c r="J8">
-        <v>100</v>
-      </c>
-      <c r="K8" t="s">
-        <v>37</v>
-      </c>
-      <c r="L8">
-        <v>11</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8" t="s">
-        <v>22</v>
-      </c>
-      <c r="O8">
-        <v>3</v>
-      </c>
-      <c r="P8" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:16">
@@ -1015,40 +1024,40 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9">
+        <v>11</v>
+      </c>
+      <c r="G9" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9">
+        <v>22</v>
+      </c>
+      <c r="I9" t="s">
         <v>34</v>
       </c>
-      <c r="F9">
-        <v>8</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="J9">
+        <v>100</v>
+      </c>
+      <c r="K9" t="s">
         <v>35</v>
       </c>
-      <c r="H9">
-        <v>10</v>
-      </c>
-      <c r="I9" t="s">
+      <c r="L9">
+        <v>23</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9" t="s">
+        <v>22</v>
+      </c>
+      <c r="O9">
+        <v>3</v>
+      </c>
+      <c r="P9" t="s">
         <v>36</v>
-      </c>
-      <c r="J9">
-        <v>100</v>
-      </c>
-      <c r="K9" t="s">
-        <v>37</v>
-      </c>
-      <c r="L9">
-        <v>11</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9" t="s">
-        <v>22</v>
-      </c>
-      <c r="O9">
-        <v>3</v>
-      </c>
-      <c r="P9" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -1065,25 +1074,25 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F10">
         <v>9</v>
       </c>
       <c r="G10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H10">
         <v>9</v>
       </c>
       <c r="I10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J10">
         <v>100</v>
       </c>
       <c r="K10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L10">
         <v>10</v>
@@ -1098,7 +1107,7 @@
         <v>3</v>
       </c>
       <c r="P10" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -1115,25 +1124,25 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F11">
         <v>9</v>
       </c>
       <c r="G11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H11">
         <v>9</v>
       </c>
       <c r="I11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J11">
         <v>100</v>
       </c>
       <c r="K11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L11">
         <v>10</v>
@@ -1148,7 +1157,7 @@
         <v>3</v>
       </c>
       <c r="P11" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -1156,7 +1165,7 @@
         <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12">
         <v>0.2</v>
@@ -1165,19 +1174,19 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F12">
         <v>7</v>
       </c>
       <c r="G12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H12">
         <v>49</v>
       </c>
       <c r="I12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J12">
         <v>100</v>
@@ -1198,7 +1207,7 @@
         <v>3</v>
       </c>
       <c r="P12" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -1206,7 +1215,7 @@
         <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13">
         <v>0.2</v>
@@ -1215,19 +1224,19 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F13">
         <v>7</v>
       </c>
       <c r="G13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H13">
         <v>49</v>
       </c>
       <c r="I13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J13">
         <v>100</v>
@@ -1248,7 +1257,7 @@
         <v>3</v>
       </c>
       <c r="P13" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -1256,7 +1265,7 @@
         <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14">
         <v>0.4</v>
@@ -1268,13 +1277,13 @@
         <v>47</v>
       </c>
       <c r="F14">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G14" t="s">
         <v>48</v>
       </c>
       <c r="H14">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="I14" t="s">
         <v>49</v>
@@ -1283,11 +1292,11 @@
         <v>100</v>
       </c>
       <c r="K14" t="s">
+        <v>21</v>
+      </c>
+      <c r="L14">
         <v>50</v>
       </c>
-      <c r="L14">
-        <v>19</v>
-      </c>
       <c r="M14">
         <v>0</v>
       </c>
@@ -1298,7 +1307,7 @@
         <v>3</v>
       </c>
       <c r="P14" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -1306,7 +1315,7 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15">
         <v>0.4</v>
@@ -1318,13 +1327,13 @@
         <v>47</v>
       </c>
       <c r="F15">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G15" t="s">
         <v>48</v>
       </c>
       <c r="H15">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="I15" t="s">
         <v>49</v>
@@ -1333,11 +1342,11 @@
         <v>100</v>
       </c>
       <c r="K15" t="s">
+        <v>21</v>
+      </c>
+      <c r="L15">
         <v>50</v>
       </c>
-      <c r="L15">
-        <v>19</v>
-      </c>
       <c r="M15">
         <v>0</v>
       </c>
@@ -1348,7 +1357,7 @@
         <v>3</v>
       </c>
       <c r="P15" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:16">
@@ -1356,7 +1365,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16">
         <v>0.6</v>
@@ -1365,28 +1374,28 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16">
+        <v>9</v>
+      </c>
+      <c r="G16" t="s">
         <v>51</v>
       </c>
-      <c r="F16">
-        <v>12</v>
-      </c>
-      <c r="G16" t="s">
+      <c r="H16">
+        <v>14</v>
+      </c>
+      <c r="I16" t="s">
         <v>52</v>
       </c>
-      <c r="H16">
-        <v>27</v>
-      </c>
-      <c r="I16" t="s">
+      <c r="J16">
+        <v>100</v>
+      </c>
+      <c r="K16" t="s">
         <v>53</v>
       </c>
-      <c r="J16">
-        <v>100</v>
-      </c>
-      <c r="K16" t="s">
-        <v>54</v>
-      </c>
       <c r="L16">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="M16">
         <v>0</v>
@@ -1398,7 +1407,7 @@
         <v>3</v>
       </c>
       <c r="P16" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:16">
@@ -1406,7 +1415,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C17">
         <v>0.6</v>
@@ -1415,28 +1424,28 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17">
+        <v>9</v>
+      </c>
+      <c r="G17" t="s">
         <v>51</v>
       </c>
-      <c r="F17">
-        <v>12</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="H17">
+        <v>14</v>
+      </c>
+      <c r="I17" t="s">
         <v>52</v>
       </c>
-      <c r="H17">
-        <v>27</v>
-      </c>
-      <c r="I17" t="s">
+      <c r="J17">
+        <v>100</v>
+      </c>
+      <c r="K17" t="s">
         <v>53</v>
       </c>
-      <c r="J17">
-        <v>100</v>
-      </c>
-      <c r="K17" t="s">
-        <v>54</v>
-      </c>
       <c r="L17">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="M17">
         <v>0</v>
@@ -1448,7 +1457,7 @@
         <v>3</v>
       </c>
       <c r="P17" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:16">
@@ -1456,7 +1465,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C18">
         <v>0.8</v>
@@ -1465,28 +1474,28 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18">
+        <v>8</v>
+      </c>
+      <c r="G18" t="s">
         <v>55</v>
       </c>
-      <c r="F18">
-        <v>9</v>
-      </c>
-      <c r="G18" t="s">
+      <c r="H18">
+        <v>11</v>
+      </c>
+      <c r="I18" t="s">
         <v>56</v>
       </c>
-      <c r="H18">
-        <v>16</v>
-      </c>
-      <c r="I18" t="s">
+      <c r="J18">
+        <v>100</v>
+      </c>
+      <c r="K18" t="s">
         <v>57</v>
       </c>
-      <c r="J18">
-        <v>100</v>
-      </c>
-      <c r="K18" t="s">
-        <v>58</v>
-      </c>
       <c r="L18">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="M18">
         <v>0</v>
@@ -1498,7 +1507,7 @@
         <v>3</v>
       </c>
       <c r="P18" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:16">
@@ -1506,7 +1515,7 @@
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C19">
         <v>0.8</v>
@@ -1515,28 +1524,28 @@
         <v>1</v>
       </c>
       <c r="E19" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19">
+        <v>8</v>
+      </c>
+      <c r="G19" t="s">
         <v>55</v>
       </c>
-      <c r="F19">
-        <v>9</v>
-      </c>
-      <c r="G19" t="s">
+      <c r="H19">
+        <v>11</v>
+      </c>
+      <c r="I19" t="s">
         <v>56</v>
       </c>
-      <c r="H19">
-        <v>16</v>
-      </c>
-      <c r="I19" t="s">
+      <c r="J19">
+        <v>100</v>
+      </c>
+      <c r="K19" t="s">
         <v>57</v>
       </c>
-      <c r="J19">
-        <v>100</v>
-      </c>
-      <c r="K19" t="s">
-        <v>58</v>
-      </c>
       <c r="L19">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="M19">
         <v>0</v>
@@ -1548,7 +1557,7 @@
         <v>3</v>
       </c>
       <c r="P19" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:16">
@@ -1556,7 +1565,7 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1565,25 +1574,25 @@
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F20">
         <v>9</v>
       </c>
       <c r="G20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H20">
         <v>10</v>
       </c>
       <c r="I20" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J20">
         <v>100</v>
       </c>
       <c r="K20" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="L20">
         <v>11</v>
@@ -1598,7 +1607,7 @@
         <v>3</v>
       </c>
       <c r="P20" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -1606,7 +1615,7 @@
         <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -1615,25 +1624,25 @@
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F21">
         <v>9</v>
       </c>
       <c r="G21" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H21">
         <v>10</v>
       </c>
       <c r="I21" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J21">
         <v>100</v>
       </c>
       <c r="K21" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
       <c r="L21">
         <v>11</v>
@@ -1648,7 +1657,7 @@
         <v>3</v>
       </c>
       <c r="P21" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -1698,7 +1707,7 @@
         <v>3</v>
       </c>
       <c r="P22" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -1748,7 +1757,7 @@
         <v>3</v>
       </c>
       <c r="P23" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:16">
@@ -1774,7 +1783,7 @@
         <v>68</v>
       </c>
       <c r="H24">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I24" t="s">
         <v>69</v>
@@ -1786,7 +1795,7 @@
         <v>70</v>
       </c>
       <c r="L24">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M24">
         <v>0</v>
@@ -1798,7 +1807,7 @@
         <v>3</v>
       </c>
       <c r="P24" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:16">
@@ -1824,7 +1833,7 @@
         <v>68</v>
       </c>
       <c r="H25">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I25" t="s">
         <v>69</v>
@@ -1836,7 +1845,7 @@
         <v>70</v>
       </c>
       <c r="L25">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M25">
         <v>0</v>
@@ -1848,7 +1857,7 @@
         <v>3</v>
       </c>
       <c r="P25" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:16">
@@ -1868,25 +1877,25 @@
         <v>71</v>
       </c>
       <c r="F26">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G26" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="H26">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="I26" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J26">
         <v>100</v>
       </c>
       <c r="K26" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="L26">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="M26">
         <v>0</v>
@@ -1898,7 +1907,7 @@
         <v>3</v>
       </c>
       <c r="P26" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:16">
@@ -1918,25 +1927,25 @@
         <v>71</v>
       </c>
       <c r="F27">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G27" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="H27">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="I27" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="J27">
         <v>100</v>
       </c>
       <c r="K27" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="L27">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="M27">
         <v>0</v>
@@ -1948,7 +1957,7 @@
         <v>3</v>
       </c>
       <c r="P27" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:16">
@@ -1965,28 +1974,28 @@
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F28">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G28" t="s">
-        <v>35</v>
+        <v>75</v>
       </c>
       <c r="H28">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I28" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J28">
         <v>100</v>
       </c>
       <c r="K28" t="s">
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="L28">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="M28">
         <v>0</v>
@@ -1998,7 +2007,7 @@
         <v>3</v>
       </c>
       <c r="P28" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:16">
@@ -2015,28 +2024,28 @@
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F29">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G29" t="s">
-        <v>35</v>
+        <v>75</v>
       </c>
       <c r="H29">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="I29" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J29">
         <v>100</v>
       </c>
       <c r="K29" t="s">
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="L29">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="M29">
         <v>0</v>
@@ -2048,7 +2057,7 @@
         <v>3</v>
       </c>
       <c r="P29" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:16">
@@ -2065,25 +2074,25 @@
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F30">
         <v>9</v>
       </c>
       <c r="G30" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H30">
         <v>9</v>
       </c>
       <c r="I30" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J30">
         <v>100</v>
       </c>
       <c r="K30" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L30">
         <v>10</v>
@@ -2098,7 +2107,7 @@
         <v>3</v>
       </c>
       <c r="P30" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
     </row>
     <row r="31" spans="1:16">
@@ -2115,25 +2124,25 @@
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F31">
         <v>9</v>
       </c>
       <c r="G31" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H31">
         <v>9</v>
       </c>
       <c r="I31" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J31">
         <v>100</v>
       </c>
       <c r="K31" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L31">
         <v>10</v>
@@ -2148,7 +2157,7 @@
         <v>3</v>
       </c>
       <c r="P31" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>